<commit_message>
Merged PR 11409: Update provider id range max value
Update provider id range max value

Related work items: #62954
</commit_message>
<xml_diff>
--- a/CalculateFunding.Services.Datasets.UnitTests/TestItems/Factors_DoNotValidateProviders_VariousInvalidFields.xlsx
+++ b/CalculateFunding.Services.Datasets.UnitTests/TestItems/Factors_DoNotValidateProviders_VariousInvalidFields.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23901"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\src\sinem\CalculateFunding-Backend\CalculateFunding.Services.Datasets.UnitTests\TestItems\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17D07878-FD8B-464C-8A86-893A4743592A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{86FE68C8-6153-450C-BC64-863922BB9178}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21220" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="7210" yWindow="970" windowWidth="28800" windowHeight="15290" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Factors" sheetId="1" r:id="rId1"/>
@@ -142,7 +142,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="13">
   <si>
     <t>Provider Name</t>
   </si>
@@ -511,10 +511,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I3"/>
+  <dimension ref="A1:I4"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.5"/>
@@ -617,6 +617,35 @@
         <v>2</v>
       </c>
     </row>
+    <row r="4" spans="1:9">
+      <c r="A4" s="3">
+        <v>100000001</v>
+      </c>
+      <c r="B4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D4" t="s">
+        <v>10</v>
+      </c>
+      <c r="E4">
+        <v>77.680000000000007</v>
+      </c>
+      <c r="F4">
+        <v>1.4</v>
+      </c>
+      <c r="G4">
+        <v>1</v>
+      </c>
+      <c r="H4">
+        <v>2</v>
+      </c>
+      <c r="I4">
+        <v>2</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.51180555555555596" footer="0.51180555555555596"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>